<commit_message>
Updated cost list, changes to QRPfRA class, and modifications on TROT_controller.py
</commit_message>
<xml_diff>
--- a/Parts/Parts and Material Costs.xlsx
+++ b/Parts/Parts and Material Costs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deniz/PycharmProjects/QRPfRA_Senior_Project/Parts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786AC1F9-004A-C84D-931D-48C5C7AF0D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1798CBC8-96C0-5546-9CF1-0E953558F1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22020" yWindow="3220" windowWidth="28040" windowHeight="17440" xr2:uid="{7FC9E874-0AE8-8C42-BDA3-AC4209976CB8}"/>
+    <workbookView xWindow="3040" yWindow="760" windowWidth="27180" windowHeight="18880" xr2:uid="{7FC9E874-0AE8-8C42-BDA3-AC4209976CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,18 +36,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Parts</t>
-  </si>
-  <si>
-    <t>Cost</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Piece(s)</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4B - 8Gb</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Camera Module 3</t>
+  </si>
+  <si>
+    <t>MG996R Servo</t>
+  </si>
+  <si>
+    <t>1Kg PLA+ 3D Printer Filament</t>
+  </si>
+  <si>
+    <t>Adafruit BNO055 9-DOF IMU</t>
+  </si>
+  <si>
+    <t>Custom Designed PCB</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>TAIYO YUDEN TMK316BJ106ML-T Cap, 10Âµf, 25V, 20%, X5r, 1206</t>
+  </si>
+  <si>
+    <t>TAIYO YUDEN TMK316BBJ226ML-T Capacitor, Mlcc, X5r, 22Uf, 25V, 1206</t>
+  </si>
+  <si>
+    <t>KEMET C0603C104M5RACTU Cap, 0.1Âµf, 50V, 20%, X7r, 0603</t>
+  </si>
+  <si>
+    <t>WALSIN WR06X104 JTL Res, 100K, 5%, 0.1W, 0603, Thick Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VISHAY CRCW060352K3FKEA. Res, 52K3, 1%, 0.1W, 0603, Thick Film</t>
+  </si>
+  <si>
+    <t>BOURNS CR0603-FX-1002ELF Res, 10K, 1%, 0.1W, 0603, Thick Film</t>
+  </si>
+  <si>
+    <t>MULTICOMP PRO MCWR06X102 JTL Res, 1K, 5%, 0.1W, 0603, Thick Film</t>
+  </si>
+  <si>
+    <t>TDK VLS6045EX-3R3N Inductor, 3.3Uh, 4.95A, 30%, Wirewound</t>
+  </si>
+  <si>
+    <t>Diodes Inc AP62300Z6-7 DcDc Conv Sync Buck 750Khz 85Deg C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Multicomp Pro MP008288 Led Green 90Mcd 577Nm 0603</t>
+  </si>
+  <si>
+    <t>Multicomp Pro MP011984 Tb Wire To Brd RA 2Way 18Awg</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 2x20 Header Pin</t>
+  </si>
+  <si>
+    <t>1x40 180 Degree Female Header</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>21700 Li-Ion Battery</t>
+  </si>
+  <si>
+    <t>3S 60A BMS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$₺-41F]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;₺&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -57,16 +130,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -78,7 +151,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -86,19 +159,127 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;₺&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -109,6 +290,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EDE72D0D-CD35-424D-9E79-50FD08714D39}" name="Table1" displayName="Table1" ref="A1:C23" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:C23" xr:uid="{EDE72D0D-CD35-424D-9E79-50FD08714D39}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{4C730C9C-1A24-C14B-9702-3A6897380122}" name="Part" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{85B2CEF0-ACCD-AB49-A05B-FE2817DA5E89}" name="Piece(s)"/>
+    <tableColumn id="3" xr3:uid="{E8CF3AC2-985A-5C4F-8ED8-6DFDEADC641A}" name="Total Cost" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,27 +621,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9168508-F95B-484B-A2D9-E6441AB05698}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2958.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>889.93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6">
+        <v>882.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>445.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1577.56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
+        <v>374.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6">
+        <f>D8+D8*20%</f>
+        <v>48.611999999999995</v>
+      </c>
+      <c r="D8">
+        <v>40.51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="9">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" ref="C9:C18" si="0">D9+D9*20%</f>
+        <v>127.36799999999999</v>
+      </c>
+      <c r="D9">
+        <v>106.14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="0"/>
+        <v>8.4719999999999995</v>
+      </c>
+      <c r="D10">
+        <v>7.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="0"/>
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="D11">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="0"/>
+        <v>10.704000000000001</v>
+      </c>
+      <c r="D12">
+        <v>8.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="0"/>
+        <v>4.008</v>
+      </c>
+      <c r="D13">
+        <v>3.34</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="0"/>
+        <v>2.2679999999999998</v>
+      </c>
+      <c r="D14">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="9">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="0"/>
+        <v>70.512</v>
+      </c>
+      <c r="D15">
+        <v>58.76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="9">
+        <v>10</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>127.32</v>
+      </c>
+      <c r="D16">
+        <f>53.05*2</f>
+        <v>106.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="9">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>19.404000000000003</v>
+      </c>
+      <c r="D17">
+        <v>16.170000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="9">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>47.628</v>
+      </c>
+      <c r="D18">
+        <v>39.69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>43.16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="9">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="9">
+        <v>3</v>
+      </c>
+      <c r="C21" s="7">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7">
+        <v>231.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="14">
+        <f>SUM(C2:C22)</f>
+        <v>8837.9359999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
+      <c r="C24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modification to XML models
</commit_message>
<xml_diff>
--- a/Parts/Parts and Material Costs.xlsx
+++ b/Parts/Parts and Material Costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deniz/PycharmProjects/QRPfRA_Senior_Project/Parts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1798CBC8-96C0-5546-9CF1-0E953558F1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205CD84A-09AC-6148-B5B5-F79B60C42E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="760" windowWidth="27180" windowHeight="18880" xr2:uid="{7FC9E874-0AE8-8C42-BDA3-AC4209976CB8}"/>
   </bookViews>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9168508-F95B-484B-A2D9-E6441AB05698}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="134" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C23" sqref="A1:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,7 +635,7 @@
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -646,7 +646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -657,7 +657,7 @@
         <v>2958.75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -668,7 +668,7 @@
         <v>889.93</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -679,7 +679,7 @@
         <v>882.4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -690,7 +690,7 @@
         <v>445.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -701,7 +701,7 @@
         <v>1577.56</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -712,7 +712,7 @@
         <v>374.92</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -727,7 +727,7 @@
         <v>40.51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -742,7 +742,7 @@
         <v>106.14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -757,7 +757,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -772,7 +772,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -787,7 +787,7 @@
         <v>8.92</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -803,7 +803,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -818,7 +818,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -833,7 +833,7 @@
         <v>58.76</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -849,7 +849,7 @@
         <v>106.1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -864,7 +864,7 @@
         <v>16.170000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -879,7 +879,7 @@
         <v>39.69</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
@@ -890,7 +890,7 @@
         <v>43.16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
@@ -901,7 +901,7 @@
         <v>5.49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -912,7 +912,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -923,7 +923,7 @@
         <v>231.95</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>22</v>

</xml_diff>